<commit_message>
Save and reload file before testing. Conditional formats don't work exactly as planned yet.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/StyleReferenceFiles/TransparentBackgroundFill/TransparentBackgroundFill.xlsx
+++ b/ClosedXML_Tests/Resource/StyleReferenceFiles/TransparentBackgroundFill/TransparentBackgroundFill.xlsx
@@ -158,10 +158,7 @@
         <x:color theme="1"/>
       </x:font>
       <x:fill>
-        <x:patternFill patternType="solid">
-          <x:fgColor auto="1"/>
-          <x:bgColor/>
-        </x:patternFill>
+        <x:patternFill patternType="none"/>
       </x:fill>
     </x:dxf>
   </x:dxfs>
@@ -484,24 +481,50 @@
     <x:col min="2" max="16384" width="9" style="4" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="2" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="3" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="4" spans="1:1" customFormat="1" ht="18" customHeight="1">
+    <x:row r="1" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A1" s="3" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A2" s="3" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A3" s="3" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
       <x:c r="A4" s="4" t="n">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="6" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="7" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="8" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="9" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="10" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="11" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="12" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="13" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
-    <x:row r="14" spans="1:1" customFormat="1" ht="18" customHeight="1"/>
+    <x:row r="5" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A5" s="3" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A6" s="3" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A7" s="3" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A8" s="3" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A9" s="3" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A10" s="3" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A11" s="3" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A12" s="3" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A13" s="3" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:1" s="3" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A14" s="3" t="s"/>
+    </x:row>
   </x:sheetData>
   <x:phoneticPr fontId="1" type="noConversion"/>
   <x:conditionalFormatting sqref="A1:A7">

</xml_diff>